<commit_message>
Update several PRQL queries; Add data for current 2024 GCRoD entries
</commit_message>
<xml_diff>
--- a/RawData/Lyme Zoning Permits-2016-2022-RB multi Year.xlsx
+++ b/RawData/Lyme Zoning Permits-2016-2022-RB multi Year.xlsx
@@ -1,30 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richb/github/TaxFairness/Raw Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richb/github/TaxFairness/RawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E77284-E16D-864E-B7D1-F2229956E3E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26973683-95A1-4A44-88F0-9E2A4F370194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2080" windowWidth="24980" windowHeight="9960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="2080" windowWidth="27040" windowHeight="16660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lyme Zoning Permits-RAW" sheetId="1" r:id="rId1"/>
     <sheet name="Lyme Zoning Permits-Processed" sheetId="2" r:id="rId2"/>
-    <sheet name="Zoning Permits 2022-mid-2023" sheetId="3" r:id="rId3"/>
+    <sheet name="New Residences" sheetId="4" r:id="rId3"/>
+    <sheet name="Zoning Permits 2022-mid-2023" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3609" uniqueCount="1431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3689" uniqueCount="1434">
   <si>
     <t>2016-04</t>
   </si>
@@ -4326,6 +4329,15 @@
   </si>
   <si>
     <t>Duplicate</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t># New Units</t>
+  </si>
+  <si>
+    <t>Between Sep 2016 and Sep 2022, there were 16 new units permitted; that's 2.7 units per year.</t>
   </si>
 </sst>
 </file>
@@ -16423,8 +16435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M435"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16433,7 +16445,7 @@
     <col min="3" max="3" width="13.33203125" style="4" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
     <col min="9" max="9" width="23.5" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" customWidth="1"/>
+    <col min="10" max="10" width="44.83203125" customWidth="1"/>
     <col min="11" max="11" width="10.83203125" style="5"/>
     <col min="12" max="12" width="10.83203125" style="4"/>
   </cols>
@@ -16484,34 +16496,38 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>42395</v>
+        <v>42397</v>
       </c>
       <c r="C2" s="4">
-        <v>42396</v>
+        <v>42397</v>
       </c>
       <c r="D2">
-        <v>201</v>
+        <v>408</v>
       </c>
       <c r="E2">
-        <v>133</v>
+        <v>59</v>
       </c>
       <c r="F2">
-        <v>133</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K2" s="5">
-        <v>10000</v>
+        <v>15</v>
       </c>
       <c r="L2" s="4">
         <v>43831</v>
+      </c>
+      <c r="M2" t="str">
+        <f>IF(A1=A2,"dup","")</f>
+        <v/>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -16519,38 +16535,34 @@
         <v>0</v>
       </c>
       <c r="B3" s="4">
-        <v>42397</v>
+        <v>42395</v>
       </c>
       <c r="C3" s="4">
-        <v>42397</v>
+        <v>42396</v>
       </c>
       <c r="D3">
-        <v>408</v>
+        <v>201</v>
       </c>
       <c r="E3">
-        <v>59</v>
+        <v>133</v>
       </c>
       <c r="F3">
-        <v>59</v>
+        <v>133</v>
       </c>
       <c r="H3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K3" s="5">
-        <v>15</v>
+        <v>10000</v>
       </c>
       <c r="L3" s="4">
         <v>43831</v>
-      </c>
-      <c r="M3" t="str">
-        <f>IF(A2=A3,"dup","")</f>
-        <v>dup</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -16588,7 +16600,7 @@
         <v>43831</v>
       </c>
       <c r="M4" t="str">
-        <f t="shared" ref="M4:M67" si="0">IF(A3=A4,"dup","")</f>
+        <f>IF(A3=A4,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -16627,7 +16639,7 @@
         <v>43831</v>
       </c>
       <c r="M5" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A4=A5,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -16666,7 +16678,7 @@
         <v>43831</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A5=A6,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -16705,7 +16717,7 @@
         <v>43831</v>
       </c>
       <c r="M7" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A6=A7,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -16744,7 +16756,7 @@
         <v>43831</v>
       </c>
       <c r="M8" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A7=A8,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -16783,7 +16795,7 @@
         <v>43831</v>
       </c>
       <c r="M9" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A8=A9,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -16822,7 +16834,7 @@
         <v>43831</v>
       </c>
       <c r="M10" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A9=A10,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -16861,7 +16873,7 @@
         <v>43831</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A10=A11,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -16903,7 +16915,7 @@
         <v>43831</v>
       </c>
       <c r="M12" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A11=A12,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -16912,37 +16924,37 @@
         <v>35</v>
       </c>
       <c r="B13" s="4">
-        <v>42461</v>
+        <v>42481</v>
       </c>
       <c r="C13" s="4">
-        <v>42471</v>
+        <v>42481</v>
       </c>
       <c r="D13">
-        <v>413</v>
+        <v>201</v>
       </c>
       <c r="E13">
+        <v>75</v>
+      </c>
+      <c r="F13">
         <v>9</v>
       </c>
-      <c r="F13">
-        <v>75</v>
-      </c>
       <c r="H13" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="I13" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="J13" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="K13" s="5">
-        <v>62000</v>
+        <v>15</v>
       </c>
       <c r="L13" s="4">
         <v>43831</v>
       </c>
       <c r="M13" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A12=A13,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -16951,37 +16963,37 @@
         <v>35</v>
       </c>
       <c r="B14" s="4">
-        <v>42481</v>
+        <v>42461</v>
       </c>
       <c r="C14" s="4">
-        <v>42481</v>
+        <v>42471</v>
       </c>
       <c r="D14">
-        <v>201</v>
+        <v>413</v>
       </c>
       <c r="E14">
+        <v>9</v>
+      </c>
+      <c r="F14">
         <v>75</v>
       </c>
-      <c r="F14">
-        <v>9</v>
-      </c>
       <c r="H14" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I14" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="J14" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="K14" s="5">
-        <v>15</v>
+        <v>62000</v>
       </c>
       <c r="L14" s="4">
         <v>43831</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A13=A14,"dup","")</f>
         <v>dup</v>
       </c>
     </row>
@@ -17023,7 +17035,7 @@
         <v>43831</v>
       </c>
       <c r="M15" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A14=A15,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17062,7 +17074,7 @@
         <v>43831</v>
       </c>
       <c r="M16" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A15=A16,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17104,7 +17116,7 @@
         <v>43831</v>
       </c>
       <c r="M17" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A16=A17,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17143,7 +17155,7 @@
         <v>43831</v>
       </c>
       <c r="M18" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A17=A18,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17182,7 +17194,7 @@
         <v>43831</v>
       </c>
       <c r="M19" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A18=A19,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17221,7 +17233,7 @@
         <v>43831</v>
       </c>
       <c r="M20" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A19=A20,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17260,7 +17272,7 @@
         <v>43831</v>
       </c>
       <c r="M21" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A20=A21,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17299,7 +17311,7 @@
         <v>43831</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A21=A22,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17338,7 +17350,7 @@
         <v>43831</v>
       </c>
       <c r="M23" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A22=A23,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17377,7 +17389,7 @@
         <v>43831</v>
       </c>
       <c r="M24" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A23=A24,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17416,7 +17428,7 @@
         <v>43831</v>
       </c>
       <c r="M25" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A24=A25,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17458,7 +17470,7 @@
         <v>43831</v>
       </c>
       <c r="M26" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A25=A26,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17497,7 +17509,7 @@
         <v>43831</v>
       </c>
       <c r="M27" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A26=A27,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17536,7 +17548,7 @@
         <v>43831</v>
       </c>
       <c r="M28" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A27=A28,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17575,7 +17587,7 @@
         <v>43831</v>
       </c>
       <c r="M29" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A28=A29,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17614,7 +17626,7 @@
         <v>43831</v>
       </c>
       <c r="M30" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A29=A30,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17653,7 +17665,7 @@
         <v>43831</v>
       </c>
       <c r="M31" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A30=A31,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17692,7 +17704,7 @@
         <v>43831</v>
       </c>
       <c r="M32" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A31=A32,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17731,7 +17743,7 @@
         <v>43831</v>
       </c>
       <c r="M33" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A32=A33,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17770,7 +17782,7 @@
         <v>43831</v>
       </c>
       <c r="M34" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A33=A34,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17809,7 +17821,7 @@
         <v>43831</v>
       </c>
       <c r="M35" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A34=A35,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17848,7 +17860,7 @@
         <v>43831</v>
       </c>
       <c r="M36" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A35=A36,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17887,7 +17899,7 @@
         <v>43831</v>
       </c>
       <c r="M37" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A36=A37,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17926,7 +17938,7 @@
         <v>43831</v>
       </c>
       <c r="M38" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A37=A38,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -17962,7 +17974,7 @@
         <v>43831</v>
       </c>
       <c r="M39" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A38=A39,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18004,7 +18016,7 @@
         <v>43831</v>
       </c>
       <c r="M40" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A39=A40,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18043,7 +18055,7 @@
         <v>43831</v>
       </c>
       <c r="M41" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A40=A41,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18085,7 +18097,7 @@
         <v>43831</v>
       </c>
       <c r="M42" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A41=A42,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18124,7 +18136,7 @@
         <v>43831</v>
       </c>
       <c r="M43" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A42=A43,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18163,7 +18175,7 @@
         <v>43831</v>
       </c>
       <c r="M44" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A43=A44,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18205,7 +18217,7 @@
         <v>43831</v>
       </c>
       <c r="M45" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A44=A45,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18247,7 +18259,7 @@
         <v>43831</v>
       </c>
       <c r="M46" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A45=A46,"dup","")</f>
         <v>dup</v>
       </c>
     </row>
@@ -18289,7 +18301,7 @@
         <v>43831</v>
       </c>
       <c r="M47" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A46=A47,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18328,7 +18340,7 @@
         <v>43831</v>
       </c>
       <c r="M48" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A47=A48,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18367,7 +18379,7 @@
         <v>43831</v>
       </c>
       <c r="M49" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A48=A49,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18406,7 +18418,7 @@
         <v>43831</v>
       </c>
       <c r="M50" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A49=A50,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18445,7 +18457,7 @@
         <v>43831</v>
       </c>
       <c r="M51" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A50=A51,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18484,7 +18496,7 @@
         <v>43831</v>
       </c>
       <c r="M52" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A51=A52,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18523,7 +18535,7 @@
         <v>43831</v>
       </c>
       <c r="M53" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A52=A53,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18562,7 +18574,7 @@
         <v>43831</v>
       </c>
       <c r="M54" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A53=A54,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18601,7 +18613,7 @@
         <v>43831</v>
       </c>
       <c r="M55" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A54=A55,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18640,7 +18652,7 @@
         <v>43831</v>
       </c>
       <c r="M56" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A55=A56,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18679,7 +18691,7 @@
         <v>43831</v>
       </c>
       <c r="M57" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A56=A57,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18718,7 +18730,7 @@
         <v>43831</v>
       </c>
       <c r="M58" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A57=A58,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18757,7 +18769,7 @@
         <v>43831</v>
       </c>
       <c r="M59" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A58=A59,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18796,7 +18808,7 @@
         <v>43831</v>
       </c>
       <c r="M60" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A59=A60,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18835,7 +18847,7 @@
         <v>43831</v>
       </c>
       <c r="M61" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A60=A61,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18874,7 +18886,7 @@
         <v>43831</v>
       </c>
       <c r="M62" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A61=A62,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18913,7 +18925,7 @@
         <v>43831</v>
       </c>
       <c r="M63" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A62=A63,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18952,7 +18964,7 @@
         <v>43831</v>
       </c>
       <c r="M64" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A63=A64,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -18991,7 +19003,7 @@
         <v>43831</v>
       </c>
       <c r="M65" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A64=A65,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19030,7 +19042,7 @@
         <v>43831</v>
       </c>
       <c r="M66" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A65=A66,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19069,7 +19081,7 @@
         <v>43831</v>
       </c>
       <c r="M67" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(A66=A67,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19111,7 +19123,7 @@
         <v>43831</v>
       </c>
       <c r="M68" t="str">
-        <f t="shared" ref="M68:M131" si="1">IF(A67=A68,"dup","")</f>
+        <f>IF(A67=A68,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19150,7 +19162,7 @@
         <v>43831</v>
       </c>
       <c r="M69" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A68=A69,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19192,7 +19204,7 @@
         <v>43831</v>
       </c>
       <c r="M70" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A69=A70,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19231,7 +19243,7 @@
         <v>43831</v>
       </c>
       <c r="M71" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A70=A71,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19273,7 +19285,7 @@
         <v>43831</v>
       </c>
       <c r="M72" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A71=A72,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19312,7 +19324,7 @@
         <v>43831</v>
       </c>
       <c r="M73" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A72=A73,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19351,7 +19363,7 @@
         <v>43831</v>
       </c>
       <c r="M74" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A73=A74,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19393,7 +19405,7 @@
         <v>43831</v>
       </c>
       <c r="M75" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A74=A75,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19432,7 +19444,7 @@
         <v>43831</v>
       </c>
       <c r="M76" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A75=A76,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19471,7 +19483,7 @@
         <v>43831</v>
       </c>
       <c r="M77" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A76=A77,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19510,7 +19522,7 @@
         <v>43831</v>
       </c>
       <c r="M78" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A77=A78,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19549,7 +19561,7 @@
         <v>43831</v>
       </c>
       <c r="M79" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A78=A79,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19591,7 +19603,7 @@
         <v>43831</v>
       </c>
       <c r="M80" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A79=A80,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19630,7 +19642,7 @@
         <v>43831</v>
       </c>
       <c r="M81" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A80=A81,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19669,7 +19681,7 @@
         <v>43831</v>
       </c>
       <c r="M82" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A81=A82,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19708,7 +19720,7 @@
         <v>43831</v>
       </c>
       <c r="M83" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A82=A83,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19747,7 +19759,7 @@
         <v>43831</v>
       </c>
       <c r="M84" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A83=A84,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19786,7 +19798,7 @@
         <v>43831</v>
       </c>
       <c r="M85" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A84=A85,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19828,7 +19840,7 @@
         <v>43831</v>
       </c>
       <c r="M86" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A85=A86,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19867,7 +19879,7 @@
         <v>43831</v>
       </c>
       <c r="M87" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A86=A87,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19906,7 +19918,7 @@
         <v>43831</v>
       </c>
       <c r="M88" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A87=A88,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19945,7 +19957,7 @@
         <v>43831</v>
       </c>
       <c r="M89" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A88=A89,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -19984,7 +19996,7 @@
         <v>43831</v>
       </c>
       <c r="M90" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A89=A90,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20023,7 +20035,7 @@
         <v>43831</v>
       </c>
       <c r="M91" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A90=A91,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20062,7 +20074,7 @@
         <v>43831</v>
       </c>
       <c r="M92" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A91=A92,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20101,7 +20113,7 @@
         <v>43831</v>
       </c>
       <c r="M93" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A92=A93,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20140,7 +20152,7 @@
         <v>43831</v>
       </c>
       <c r="M94" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A93=A94,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20149,37 +20161,37 @@
         <v>348</v>
       </c>
       <c r="B95" s="4">
-        <v>43021</v>
+        <v>43038</v>
       </c>
       <c r="C95" s="4">
-        <v>43026</v>
+        <v>43038</v>
       </c>
       <c r="D95">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="E95">
+        <v>39</v>
+      </c>
+      <c r="F95">
         <v>50</v>
       </c>
-      <c r="F95">
-        <v>39</v>
-      </c>
       <c r="H95" t="s">
-        <v>351</v>
+        <v>116</v>
       </c>
       <c r="I95" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="J95" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="K95" s="5">
-        <v>15000</v>
+        <v>15</v>
       </c>
       <c r="L95" s="4">
         <v>43831</v>
       </c>
       <c r="M95" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A94=A95,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20188,37 +20200,37 @@
         <v>348</v>
       </c>
       <c r="B96" s="4">
-        <v>43038</v>
+        <v>43021</v>
       </c>
       <c r="C96" s="4">
-        <v>43038</v>
+        <v>43026</v>
       </c>
       <c r="D96">
-        <v>401</v>
+        <v>409</v>
       </c>
       <c r="E96">
+        <v>50</v>
+      </c>
+      <c r="F96">
         <v>39</v>
       </c>
-      <c r="F96">
-        <v>50</v>
-      </c>
       <c r="H96" t="s">
-        <v>116</v>
+        <v>351</v>
       </c>
       <c r="I96" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="J96" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="K96" s="5">
-        <v>15</v>
+        <v>15000</v>
       </c>
       <c r="L96" s="4">
         <v>43831</v>
       </c>
       <c r="M96" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A95=A96,"dup","")</f>
         <v>dup</v>
       </c>
     </row>
@@ -20260,7 +20272,7 @@
         <v>43831</v>
       </c>
       <c r="M97" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A96=A97,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20299,7 +20311,7 @@
         <v>43831</v>
       </c>
       <c r="M98" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A97=A98,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20338,7 +20350,7 @@
         <v>43831</v>
       </c>
       <c r="M99" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A98=A99,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20377,7 +20389,7 @@
         <v>43831</v>
       </c>
       <c r="M100" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A99=A100,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20419,7 +20431,7 @@
         <v>43831</v>
       </c>
       <c r="M101" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A100=A101,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20458,7 +20470,7 @@
         <v>43831</v>
       </c>
       <c r="M102" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A101=A102,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20500,7 +20512,7 @@
         <v>43831</v>
       </c>
       <c r="M103" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A102=A103,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20539,7 +20551,7 @@
         <v>43831</v>
       </c>
       <c r="M104" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A103=A104,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20578,7 +20590,7 @@
         <v>43831</v>
       </c>
       <c r="M105" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A104=A105,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20620,7 +20632,7 @@
         <v>43831</v>
       </c>
       <c r="M106" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A105=A106,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20662,7 +20674,7 @@
         <v>43831</v>
       </c>
       <c r="M107" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A106=A107,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20701,7 +20713,7 @@
         <v>43831</v>
       </c>
       <c r="M108" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A107=A108,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20743,7 +20755,7 @@
         <v>43831</v>
       </c>
       <c r="M109" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A108=A109,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20782,7 +20794,7 @@
         <v>43831</v>
       </c>
       <c r="M110" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A109=A110,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20821,7 +20833,7 @@
         <v>43831</v>
       </c>
       <c r="M111" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A110=A111,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20860,7 +20872,7 @@
         <v>43831</v>
       </c>
       <c r="M112" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A111=A112,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20902,7 +20914,7 @@
         <v>43831</v>
       </c>
       <c r="M113" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A112=A113,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20941,7 +20953,7 @@
         <v>43831</v>
       </c>
       <c r="M114" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A113=A114,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -20980,7 +20992,7 @@
         <v>43831</v>
       </c>
       <c r="M115" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A114=A115,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21019,7 +21031,7 @@
         <v>43831</v>
       </c>
       <c r="M116" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A115=A116,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21061,7 +21073,7 @@
         <v>43831</v>
       </c>
       <c r="M117" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A116=A117,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21100,7 +21112,7 @@
         <v>43831</v>
       </c>
       <c r="M118" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A117=A118,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21139,7 +21151,7 @@
         <v>43831</v>
       </c>
       <c r="M119" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A118=A119,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21181,7 +21193,7 @@
         <v>43831</v>
       </c>
       <c r="M120" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A119=A120,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21220,7 +21232,7 @@
         <v>43831</v>
       </c>
       <c r="M121" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A120=A121,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21259,7 +21271,7 @@
         <v>43831</v>
       </c>
       <c r="M122" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A121=A122,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21298,7 +21310,7 @@
         <v>43831</v>
       </c>
       <c r="M123" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A122=A123,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21337,7 +21349,7 @@
         <v>43831</v>
       </c>
       <c r="M124" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A123=A124,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21376,7 +21388,7 @@
         <v>43831</v>
       </c>
       <c r="M125" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A124=A125,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21415,7 +21427,7 @@
         <v>43831</v>
       </c>
       <c r="M126" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A125=A126,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21454,7 +21466,7 @@
         <v>43831</v>
       </c>
       <c r="M127" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A126=A127,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21493,7 +21505,7 @@
         <v>43831</v>
       </c>
       <c r="M128" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A127=A128,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21532,7 +21544,7 @@
         <v>43831</v>
       </c>
       <c r="M129" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A128=A129,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21571,7 +21583,7 @@
         <v>43831</v>
       </c>
       <c r="M130" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A129=A130,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21613,7 +21625,7 @@
         <v>43831</v>
       </c>
       <c r="M131" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(A130=A131,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21652,7 +21664,7 @@
         <v>43831</v>
       </c>
       <c r="M132" t="str">
-        <f t="shared" ref="M132:M195" si="2">IF(A131=A132,"dup","")</f>
+        <f>IF(A131=A132,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21691,7 +21703,7 @@
         <v>43831</v>
       </c>
       <c r="M133" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A132=A133,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21730,7 +21742,7 @@
         <v>43831</v>
       </c>
       <c r="M134" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A133=A134,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21769,7 +21781,7 @@
         <v>43831</v>
       </c>
       <c r="M135" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A134=A135,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21808,7 +21820,7 @@
         <v>43831</v>
       </c>
       <c r="M136" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A135=A136,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21850,7 +21862,7 @@
         <v>43831</v>
       </c>
       <c r="M137" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A136=A137,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21889,7 +21901,7 @@
         <v>43831</v>
       </c>
       <c r="M138" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A137=A138,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21928,7 +21940,7 @@
         <v>43831</v>
       </c>
       <c r="M139" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A138=A139,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -21967,7 +21979,7 @@
         <v>43831</v>
       </c>
       <c r="M140" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A139=A140,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22006,7 +22018,7 @@
         <v>43831</v>
       </c>
       <c r="M141" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A140=A141,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22045,7 +22057,7 @@
         <v>43831</v>
       </c>
       <c r="M142" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A141=A142,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22087,7 +22099,7 @@
         <v>43831</v>
       </c>
       <c r="M143" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A142=A143,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22126,7 +22138,7 @@
         <v>43831</v>
       </c>
       <c r="M144" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A143=A144,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22168,7 +22180,7 @@
         <v>43831</v>
       </c>
       <c r="M145" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A144=A145,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22207,7 +22219,7 @@
         <v>43831</v>
       </c>
       <c r="M146" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A145=A146,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22246,7 +22258,7 @@
         <v>43831</v>
       </c>
       <c r="M147" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A146=A147,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22285,7 +22297,7 @@
         <v>43831</v>
       </c>
       <c r="M148" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A147=A148,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22324,7 +22336,7 @@
         <v>43831</v>
       </c>
       <c r="M149" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A148=A149,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22363,7 +22375,7 @@
         <v>43831</v>
       </c>
       <c r="M150" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A149=A150,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22402,7 +22414,7 @@
         <v>43831</v>
       </c>
       <c r="M151" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A150=A151,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22441,7 +22453,7 @@
         <v>43831</v>
       </c>
       <c r="M152" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A151=A152,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22483,7 +22495,7 @@
         <v>43831</v>
       </c>
       <c r="M153" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A152=A153,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22522,7 +22534,7 @@
         <v>43831</v>
       </c>
       <c r="M154" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A153=A154,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22561,7 +22573,7 @@
         <v>43831</v>
       </c>
       <c r="M155" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A154=A155,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22600,7 +22612,7 @@
         <v>43831</v>
       </c>
       <c r="M156" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A155=A156,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22639,7 +22651,7 @@
         <v>43831</v>
       </c>
       <c r="M157" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A156=A157,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22681,7 +22693,7 @@
         <v>43831</v>
       </c>
       <c r="M158" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A157=A158,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22720,7 +22732,7 @@
         <v>43831</v>
       </c>
       <c r="M159" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A158=A159,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22759,7 +22771,7 @@
         <v>43831</v>
       </c>
       <c r="M160" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A159=A160,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22798,7 +22810,7 @@
         <v>43831</v>
       </c>
       <c r="M161" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A160=A161,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22840,7 +22852,7 @@
         <v>43831</v>
       </c>
       <c r="M162" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A161=A162,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22879,7 +22891,7 @@
         <v>43831</v>
       </c>
       <c r="M163" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A162=A163,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22921,7 +22933,7 @@
         <v>43831</v>
       </c>
       <c r="M164" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A163=A164,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22960,7 +22972,7 @@
         <v>43831</v>
       </c>
       <c r="M165" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A164=A165,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -22999,7 +23011,7 @@
         <v>43831</v>
       </c>
       <c r="M166" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A165=A166,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23038,7 +23050,7 @@
         <v>43831</v>
       </c>
       <c r="M167" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A166=A167,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23080,7 +23092,7 @@
         <v>43831</v>
       </c>
       <c r="M168" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A167=A168,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23119,7 +23131,7 @@
         <v>43831</v>
       </c>
       <c r="M169" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A168=A169,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23158,7 +23170,7 @@
         <v>43831</v>
       </c>
       <c r="M170" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A169=A170,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23197,7 +23209,7 @@
         <v>43831</v>
       </c>
       <c r="M171" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A170=A171,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23236,7 +23248,7 @@
         <v>43831</v>
       </c>
       <c r="M172" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A171=A172,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23275,7 +23287,7 @@
         <v>43831</v>
       </c>
       <c r="M173" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A172=A173,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23314,7 +23326,7 @@
         <v>43831</v>
       </c>
       <c r="M174" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A173=A174,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23353,7 +23365,7 @@
         <v>43831</v>
       </c>
       <c r="M175" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A174=A175,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23392,7 +23404,7 @@
         <v>43831</v>
       </c>
       <c r="M176" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A175=A176,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23431,7 +23443,7 @@
         <v>43831</v>
       </c>
       <c r="M177" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A176=A177,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23470,7 +23482,7 @@
         <v>43831</v>
       </c>
       <c r="M178" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A177=A178,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23509,7 +23521,7 @@
         <v>43831</v>
       </c>
       <c r="M179" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A178=A179,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23548,7 +23560,7 @@
         <v>43831</v>
       </c>
       <c r="M180" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A179=A180,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23587,7 +23599,7 @@
         <v>43831</v>
       </c>
       <c r="M181" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A180=A181,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23626,7 +23638,7 @@
         <v>43831</v>
       </c>
       <c r="M182" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A181=A182,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23665,7 +23677,7 @@
         <v>43831</v>
       </c>
       <c r="M183" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A182=A183,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23707,7 +23719,7 @@
         <v>43831</v>
       </c>
       <c r="M184" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A183=A184,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23746,7 +23758,7 @@
         <v>43831</v>
       </c>
       <c r="M185" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A184=A185,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23788,7 +23800,7 @@
         <v>43831</v>
       </c>
       <c r="M186" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A185=A186,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23830,7 +23842,7 @@
         <v>43831</v>
       </c>
       <c r="M187" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A186=A187,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23869,7 +23881,7 @@
         <v>43831</v>
       </c>
       <c r="M188" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A187=A188,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23908,7 +23920,7 @@
         <v>43831</v>
       </c>
       <c r="M189" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A188=A189,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23947,7 +23959,7 @@
         <v>43831</v>
       </c>
       <c r="M190" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A189=A190,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -23986,7 +23998,7 @@
         <v>43831</v>
       </c>
       <c r="M191" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A190=A191,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24025,7 +24037,7 @@
         <v>43831</v>
       </c>
       <c r="M192" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A191=A192,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24064,7 +24076,7 @@
         <v>43831</v>
       </c>
       <c r="M193" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A192=A193,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24103,7 +24115,7 @@
         <v>43831</v>
       </c>
       <c r="M194" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A193=A194,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24142,7 +24154,7 @@
         <v>43831</v>
       </c>
       <c r="M195" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(A194=A195,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24181,7 +24193,7 @@
         <v>43831</v>
       </c>
       <c r="M196" t="str">
-        <f t="shared" ref="M196:M259" si="3">IF(A195=A196,"dup","")</f>
+        <f>IF(A195=A196,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24220,7 +24232,7 @@
         <v>43831</v>
       </c>
       <c r="M197" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A196=A197,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24259,7 +24271,7 @@
         <v>43831</v>
       </c>
       <c r="M198" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A197=A198,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24298,7 +24310,7 @@
         <v>43831</v>
       </c>
       <c r="M199" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A198=A199,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24337,7 +24349,7 @@
         <v>43831</v>
       </c>
       <c r="M200" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A199=A200,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24376,7 +24388,7 @@
         <v>43831</v>
       </c>
       <c r="M201" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A200=A201,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24415,7 +24427,7 @@
         <v>43831</v>
       </c>
       <c r="M202" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A201=A202,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24454,7 +24466,7 @@
         <v>43831</v>
       </c>
       <c r="M203" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A202=A203,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24493,7 +24505,7 @@
         <v>43831</v>
       </c>
       <c r="M204" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A203=A204,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24532,7 +24544,7 @@
         <v>43831</v>
       </c>
       <c r="M205" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A204=A205,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24571,7 +24583,7 @@
         <v>43831</v>
       </c>
       <c r="M206" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A205=A206,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24610,7 +24622,7 @@
         <v>43831</v>
       </c>
       <c r="M207" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A206=A207,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24649,7 +24661,7 @@
         <v>43831</v>
       </c>
       <c r="M208" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A207=A208,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24688,7 +24700,7 @@
         <v>43831</v>
       </c>
       <c r="M209" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A208=A209,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24727,7 +24739,7 @@
         <v>43831</v>
       </c>
       <c r="M210" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A209=A210,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24766,7 +24778,7 @@
         <v>43831</v>
       </c>
       <c r="M211" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A210=A211,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24808,7 +24820,7 @@
         <v>43831</v>
       </c>
       <c r="M212" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A211=A212,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24850,7 +24862,7 @@
         <v>43831</v>
       </c>
       <c r="M213" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A212=A213,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24892,7 +24904,7 @@
         <v>43831</v>
       </c>
       <c r="M214" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A213=A214,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24931,7 +24943,7 @@
         <v>43831</v>
       </c>
       <c r="M215" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A214=A215,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -24970,7 +24982,7 @@
         <v>43831</v>
       </c>
       <c r="M216" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A215=A216,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25012,7 +25024,7 @@
         <v>43831</v>
       </c>
       <c r="M217" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A216=A217,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25051,7 +25063,7 @@
         <v>43831</v>
       </c>
       <c r="M218" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A217=A218,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25093,7 +25105,7 @@
         <v>43831</v>
       </c>
       <c r="M219" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A218=A219,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25132,7 +25144,7 @@
         <v>43831</v>
       </c>
       <c r="M220" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A219=A220,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25171,7 +25183,7 @@
         <v>43831</v>
       </c>
       <c r="M221" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A220=A221,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25210,7 +25222,7 @@
         <v>43831</v>
       </c>
       <c r="M222" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A221=A222,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25249,7 +25261,7 @@
         <v>43831</v>
       </c>
       <c r="M223" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A222=A223,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25288,7 +25300,7 @@
         <v>43831</v>
       </c>
       <c r="M224" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A223=A224,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25327,7 +25339,7 @@
         <v>43831</v>
       </c>
       <c r="M225" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A224=A225,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25366,7 +25378,7 @@
         <v>43831</v>
       </c>
       <c r="M226" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A225=A226,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25408,7 +25420,7 @@
         <v>43831</v>
       </c>
       <c r="M227" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A226=A227,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25447,7 +25459,7 @@
         <v>43831</v>
       </c>
       <c r="M228" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A227=A228,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25486,7 +25498,7 @@
         <v>43831</v>
       </c>
       <c r="M229" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A228=A229,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25525,7 +25537,7 @@
         <v>43831</v>
       </c>
       <c r="M230" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A229=A230,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25564,7 +25576,7 @@
         <v>43831</v>
       </c>
       <c r="M231" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A230=A231,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25603,7 +25615,7 @@
         <v>43831</v>
       </c>
       <c r="M232" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A231=A232,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25642,7 +25654,7 @@
         <v>43831</v>
       </c>
       <c r="M233" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A232=A233,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25681,7 +25693,7 @@
         <v>43831</v>
       </c>
       <c r="M234" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A233=A234,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25720,7 +25732,7 @@
         <v>43831</v>
       </c>
       <c r="M235" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A234=A235,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25759,7 +25771,7 @@
         <v>43831</v>
       </c>
       <c r="M236" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A235=A236,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25798,7 +25810,7 @@
         <v>43831</v>
       </c>
       <c r="M237" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A236=A237,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25837,7 +25849,7 @@
         <v>43831</v>
       </c>
       <c r="M238" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A237=A238,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25876,7 +25888,7 @@
         <v>43831</v>
       </c>
       <c r="M239" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A238=A239,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25915,7 +25927,7 @@
         <v>43831</v>
       </c>
       <c r="M240" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A239=A240,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25954,7 +25966,7 @@
         <v>43831</v>
       </c>
       <c r="M241" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A240=A241,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -25993,7 +26005,7 @@
         <v>43831</v>
       </c>
       <c r="M242" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A241=A242,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26032,7 +26044,7 @@
         <v>43831</v>
       </c>
       <c r="M243" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A242=A243,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26071,7 +26083,7 @@
         <v>43831</v>
       </c>
       <c r="M244" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A243=A244,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26110,7 +26122,7 @@
         <v>43831</v>
       </c>
       <c r="M245" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A244=A245,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26149,7 +26161,7 @@
         <v>43831</v>
       </c>
       <c r="M246" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A245=A246,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26188,7 +26200,7 @@
         <v>43831</v>
       </c>
       <c r="M247" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A246=A247,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26227,7 +26239,7 @@
         <v>43831</v>
       </c>
       <c r="M248" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A247=A248,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26266,7 +26278,7 @@
         <v>43831</v>
       </c>
       <c r="M249" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A248=A249,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26308,7 +26320,7 @@
         <v>43831</v>
       </c>
       <c r="M250" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A249=A250,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26347,7 +26359,7 @@
         <v>43831</v>
       </c>
       <c r="M251" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A250=A251,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26386,7 +26398,7 @@
         <v>43831</v>
       </c>
       <c r="M252" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A251=A252,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26425,7 +26437,7 @@
         <v>43831</v>
       </c>
       <c r="M253" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A252=A253,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26464,7 +26476,7 @@
         <v>43831</v>
       </c>
       <c r="M254" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A253=A254,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26503,7 +26515,7 @@
         <v>43831</v>
       </c>
       <c r="M255" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A254=A255,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26545,7 +26557,7 @@
         <v>43831</v>
       </c>
       <c r="M256" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A255=A256,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26584,7 +26596,7 @@
         <v>43831</v>
       </c>
       <c r="M257" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A256=A257,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26623,7 +26635,7 @@
         <v>43831</v>
       </c>
       <c r="M258" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A257=A258,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26662,7 +26674,7 @@
         <v>43831</v>
       </c>
       <c r="M259" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(A258=A259,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26701,7 +26713,7 @@
         <v>43831</v>
       </c>
       <c r="M260" t="str">
-        <f t="shared" ref="M260:M323" si="4">IF(A259=A260,"dup","")</f>
+        <f>IF(A259=A260,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26740,7 +26752,7 @@
         <v>43831</v>
       </c>
       <c r="M261" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A260=A261,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26779,7 +26791,7 @@
         <v>43831</v>
       </c>
       <c r="M262" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A261=A262,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26818,7 +26830,7 @@
         <v>43831</v>
       </c>
       <c r="M263" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A262=A263,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26857,7 +26869,7 @@
         <v>43831</v>
       </c>
       <c r="M264" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A263=A264,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26896,7 +26908,7 @@
         <v>43831</v>
       </c>
       <c r="M265" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A264=A265,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26935,7 +26947,7 @@
         <v>43831</v>
       </c>
       <c r="M266" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A265=A266,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -26974,7 +26986,7 @@
         <v>43831</v>
       </c>
       <c r="M267" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A266=A267,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27013,7 +27025,7 @@
         <v>43831</v>
       </c>
       <c r="M268" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A267=A268,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27052,7 +27064,7 @@
         <v>43831</v>
       </c>
       <c r="M269" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A268=A269,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27091,7 +27103,7 @@
         <v>43831</v>
       </c>
       <c r="M270" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A269=A270,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27130,7 +27142,7 @@
         <v>43831</v>
       </c>
       <c r="M271" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A270=A271,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27169,7 +27181,7 @@
         <v>43831</v>
       </c>
       <c r="M272" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A271=A272,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27208,7 +27220,7 @@
         <v>43831</v>
       </c>
       <c r="M273" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A272=A273,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27250,7 +27262,7 @@
         <v>43831</v>
       </c>
       <c r="M274" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A273=A274,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27292,7 +27304,7 @@
         <v>43831</v>
       </c>
       <c r="M275" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A274=A275,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27334,7 +27346,7 @@
         <v>43831</v>
       </c>
       <c r="M276" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A275=A276,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27373,7 +27385,7 @@
         <v>43831</v>
       </c>
       <c r="M277" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A276=A277,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27412,7 +27424,7 @@
         <v>43831</v>
       </c>
       <c r="M278" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A277=A278,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27451,7 +27463,7 @@
         <v>43831</v>
       </c>
       <c r="M279" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A278=A279,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27493,7 +27505,7 @@
         <v>43831</v>
       </c>
       <c r="M280" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A279=A280,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27532,7 +27544,7 @@
         <v>43831</v>
       </c>
       <c r="M281" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A280=A281,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27571,7 +27583,7 @@
         <v>43831</v>
       </c>
       <c r="M282" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A281=A282,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27613,7 +27625,7 @@
         <v>43831</v>
       </c>
       <c r="M283" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A282=A283,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27652,7 +27664,7 @@
         <v>43831</v>
       </c>
       <c r="M284" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A283=A284,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27691,7 +27703,7 @@
         <v>43831</v>
       </c>
       <c r="M285" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A284=A285,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27730,7 +27742,7 @@
         <v>43831</v>
       </c>
       <c r="M286" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A285=A286,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27769,7 +27781,7 @@
         <v>43831</v>
       </c>
       <c r="M287" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A286=A287,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27808,7 +27820,7 @@
         <v>43831</v>
       </c>
       <c r="M288" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A287=A288,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27847,7 +27859,7 @@
         <v>43831</v>
       </c>
       <c r="M289" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A288=A289,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27889,7 +27901,7 @@
         <v>43831</v>
       </c>
       <c r="M290" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A289=A290,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27931,7 +27943,7 @@
         <v>43831</v>
       </c>
       <c r="M291" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A290=A291,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -27970,7 +27982,7 @@
         <v>43831</v>
       </c>
       <c r="M292" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A291=A292,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28009,7 +28021,7 @@
         <v>43831</v>
       </c>
       <c r="M293" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A292=A293,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28048,7 +28060,7 @@
         <v>43831</v>
       </c>
       <c r="M294" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A293=A294,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28090,7 +28102,7 @@
         <v>43831</v>
       </c>
       <c r="M295" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A294=A295,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28129,7 +28141,7 @@
         <v>43831</v>
       </c>
       <c r="M296" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A295=A296,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28168,7 +28180,7 @@
         <v>43831</v>
       </c>
       <c r="M297" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A296=A297,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28207,7 +28219,7 @@
         <v>43831</v>
       </c>
       <c r="M298" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A297=A298,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28246,7 +28258,7 @@
         <v>43831</v>
       </c>
       <c r="M299" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A298=A299,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28285,7 +28297,7 @@
         <v>43831</v>
       </c>
       <c r="M300" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A299=A300,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28324,7 +28336,7 @@
         <v>43831</v>
       </c>
       <c r="M301" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A300=A301,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28363,7 +28375,7 @@
         <v>43831</v>
       </c>
       <c r="M302" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A301=A302,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28402,7 +28414,7 @@
         <v>43831</v>
       </c>
       <c r="M303" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A302=A303,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28441,7 +28453,7 @@
         <v>43831</v>
       </c>
       <c r="M304" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A303=A304,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28480,7 +28492,7 @@
         <v>43831</v>
       </c>
       <c r="M305" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A304=A305,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28519,7 +28531,7 @@
         <v>43831</v>
       </c>
       <c r="M306" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A305=A306,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28558,7 +28570,7 @@
         <v>43831</v>
       </c>
       <c r="M307" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A306=A307,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28597,7 +28609,7 @@
         <v>43831</v>
       </c>
       <c r="M308" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A307=A308,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28636,7 +28648,7 @@
         <v>43831</v>
       </c>
       <c r="M309" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A308=A309,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28675,7 +28687,7 @@
         <v>43831</v>
       </c>
       <c r="M310" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A309=A310,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28714,7 +28726,7 @@
         <v>43831</v>
       </c>
       <c r="M311" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A310=A311,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28753,7 +28765,7 @@
         <v>43831</v>
       </c>
       <c r="M312" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A311=A312,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28792,7 +28804,7 @@
         <v>43831</v>
       </c>
       <c r="M313" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A312=A313,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28831,7 +28843,7 @@
         <v>43831</v>
       </c>
       <c r="M314" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A313=A314,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28870,7 +28882,7 @@
         <v>43831</v>
       </c>
       <c r="M315" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A314=A315,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28912,7 +28924,7 @@
         <v>43831</v>
       </c>
       <c r="M316" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A315=A316,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28954,7 +28966,7 @@
         <v>43831</v>
       </c>
       <c r="M317" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A316=A317,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -28996,7 +29008,7 @@
         <v>43831</v>
       </c>
       <c r="M318" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A317=A318,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29038,7 +29050,7 @@
         <v>43831</v>
       </c>
       <c r="M319" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A318=A319,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29077,7 +29089,7 @@
         <v>43831</v>
       </c>
       <c r="M320" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A319=A320,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29116,7 +29128,7 @@
         <v>43831</v>
       </c>
       <c r="M321" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A320=A321,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29155,7 +29167,7 @@
         <v>43831</v>
       </c>
       <c r="M322" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A321=A322,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29194,7 +29206,7 @@
         <v>43831</v>
       </c>
       <c r="M323" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(A322=A323,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29233,7 +29245,7 @@
         <v>43831</v>
       </c>
       <c r="M324" t="str">
-        <f t="shared" ref="M324:M387" si="5">IF(A323=A324,"dup","")</f>
+        <f>IF(A323=A324,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29272,7 +29284,7 @@
         <v>43831</v>
       </c>
       <c r="M325" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A324=A325,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29314,7 +29326,7 @@
         <v>43831</v>
       </c>
       <c r="M326" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A325=A326,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29353,7 +29365,7 @@
         <v>43831</v>
       </c>
       <c r="M327" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A326=A327,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29395,7 +29407,7 @@
         <v>43831</v>
       </c>
       <c r="M328" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A327=A328,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29437,7 +29449,7 @@
         <v>43831</v>
       </c>
       <c r="M329" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A328=A329,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29476,7 +29488,7 @@
         <v>43831</v>
       </c>
       <c r="M330" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A329=A330,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29515,7 +29527,7 @@
         <v>43831</v>
       </c>
       <c r="M331" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A330=A331,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29554,7 +29566,7 @@
         <v>43831</v>
       </c>
       <c r="M332" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A331=A332,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29593,7 +29605,7 @@
         <v>43831</v>
       </c>
       <c r="M333" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A332=A333,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29632,7 +29644,7 @@
         <v>43831</v>
       </c>
       <c r="M334" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A333=A334,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29671,7 +29683,7 @@
         <v>43831</v>
       </c>
       <c r="M335" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A334=A335,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29710,7 +29722,7 @@
         <v>43831</v>
       </c>
       <c r="M336" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A335=A336,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29749,7 +29761,7 @@
         <v>43831</v>
       </c>
       <c r="M337" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A336=A337,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29788,7 +29800,7 @@
         <v>43831</v>
       </c>
       <c r="M338" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A337=A338,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29827,7 +29839,7 @@
         <v>43831</v>
       </c>
       <c r="M339" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A338=A339,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29866,7 +29878,7 @@
         <v>43831</v>
       </c>
       <c r="M340" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A339=A340,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29905,7 +29917,7 @@
         <v>43831</v>
       </c>
       <c r="M341" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A340=A341,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29944,7 +29956,7 @@
         <v>43831</v>
       </c>
       <c r="M342" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A341=A342,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -29983,7 +29995,7 @@
         <v>43831</v>
       </c>
       <c r="M343" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A342=A343,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30022,7 +30034,7 @@
         <v>43831</v>
       </c>
       <c r="M344" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A343=A344,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30061,7 +30073,7 @@
         <v>43831</v>
       </c>
       <c r="M345" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A344=A345,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30100,7 +30112,7 @@
         <v>43831</v>
       </c>
       <c r="M346" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A345=A346,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30139,7 +30151,7 @@
         <v>43831</v>
       </c>
       <c r="M347" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A346=A347,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30181,7 +30193,7 @@
         <v>43831</v>
       </c>
       <c r="M348" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A347=A348,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30220,7 +30232,7 @@
         <v>43831</v>
       </c>
       <c r="M349" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A348=A349,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30262,7 +30274,7 @@
         <v>43831</v>
       </c>
       <c r="M350" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A349=A350,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30304,7 +30316,7 @@
         <v>43831</v>
       </c>
       <c r="M351" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A350=A351,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30346,7 +30358,7 @@
         <v>43831</v>
       </c>
       <c r="M352" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A351=A352,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30388,7 +30400,7 @@
         <v>43831</v>
       </c>
       <c r="M353" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A352=A353,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30427,7 +30439,7 @@
         <v>43831</v>
       </c>
       <c r="M354" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A353=A354,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30466,7 +30478,7 @@
         <v>43831</v>
       </c>
       <c r="M355" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A354=A355,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30505,7 +30517,7 @@
         <v>43831</v>
       </c>
       <c r="M356" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A355=A356,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30544,7 +30556,7 @@
         <v>43831</v>
       </c>
       <c r="M357" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A356=A357,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30583,7 +30595,7 @@
         <v>43831</v>
       </c>
       <c r="M358" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A357=A358,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30622,7 +30634,7 @@
         <v>43831</v>
       </c>
       <c r="M359" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A358=A359,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30661,7 +30673,7 @@
         <v>43831</v>
       </c>
       <c r="M360" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A359=A360,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30700,7 +30712,7 @@
         <v>43831</v>
       </c>
       <c r="M361" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A360=A361,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30739,7 +30751,7 @@
         <v>43831</v>
       </c>
       <c r="M362" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A361=A362,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30778,7 +30790,7 @@
         <v>43831</v>
       </c>
       <c r="M363" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A362=A363,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30817,7 +30829,7 @@
         <v>45064</v>
       </c>
       <c r="M364" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A363=A364,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30856,7 +30868,7 @@
         <v>43831</v>
       </c>
       <c r="M365" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A364=A365,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30898,7 +30910,7 @@
         <v>43831</v>
       </c>
       <c r="M366" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A365=A366,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30937,7 +30949,7 @@
         <v>43831</v>
       </c>
       <c r="M367" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A366=A367,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -30976,7 +30988,7 @@
         <v>43831</v>
       </c>
       <c r="M368" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A367=A368,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31015,7 +31027,7 @@
         <v>43831</v>
       </c>
       <c r="M369" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A368=A369,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31054,7 +31066,7 @@
         <v>43831</v>
       </c>
       <c r="M370" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A369=A370,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31093,7 +31105,7 @@
         <v>43831</v>
       </c>
       <c r="M371" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A370=A371,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31135,7 +31147,7 @@
         <v>45064</v>
       </c>
       <c r="M372" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A371=A372,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31174,7 +31186,7 @@
         <v>43831</v>
       </c>
       <c r="M373" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A372=A373,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31213,7 +31225,7 @@
         <v>43831</v>
       </c>
       <c r="M374" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A373=A374,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31252,7 +31264,7 @@
         <v>43831</v>
       </c>
       <c r="M375" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A374=A375,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31291,7 +31303,7 @@
         <v>43831</v>
       </c>
       <c r="M376" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A375=A376,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31333,7 +31345,7 @@
         <v>43831</v>
       </c>
       <c r="M377" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A376=A377,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31372,7 +31384,7 @@
         <v>43831</v>
       </c>
       <c r="M378" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A377=A378,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31411,7 +31423,7 @@
         <v>43831</v>
       </c>
       <c r="M379" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A378=A379,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31450,7 +31462,7 @@
         <v>43831</v>
       </c>
       <c r="M380" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A379=A380,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31489,7 +31501,7 @@
         <v>43831</v>
       </c>
       <c r="M381" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A380=A381,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31528,7 +31540,7 @@
         <v>45064</v>
       </c>
       <c r="M382" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A381=A382,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31570,7 +31582,7 @@
         <v>43831</v>
       </c>
       <c r="M383" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A382=A383,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31612,7 +31624,7 @@
         <v>43831</v>
       </c>
       <c r="M384" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A383=A384,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31651,7 +31663,7 @@
         <v>43831</v>
       </c>
       <c r="M385" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A384=A385,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31690,7 +31702,7 @@
         <v>45064</v>
       </c>
       <c r="M386" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A385=A386,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31729,7 +31741,7 @@
         <v>43831</v>
       </c>
       <c r="M387" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(A386=A387,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31768,7 +31780,7 @@
         <v>43831</v>
       </c>
       <c r="M388" t="str">
-        <f t="shared" ref="M388:M404" si="6">IF(A387=A388,"dup","")</f>
+        <f>IF(A387=A388,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31807,7 +31819,7 @@
         <v>45064</v>
       </c>
       <c r="M389" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(A388=A389,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31846,7 +31858,7 @@
         <v>43831</v>
       </c>
       <c r="M390" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(A389=A390,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31885,7 +31897,7 @@
         <v>45064</v>
       </c>
       <c r="M391" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(A390=A391,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31924,7 +31936,7 @@
         <v>43831</v>
       </c>
       <c r="M392" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(A391=A392,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -31963,7 +31975,7 @@
         <v>43831</v>
       </c>
       <c r="M393" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(A392=A393,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32002,7 +32014,7 @@
         <v>43831</v>
       </c>
       <c r="M394" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(A393=A394,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32041,7 +32053,7 @@
         <v>45064</v>
       </c>
       <c r="M395" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(A394=A395,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32080,7 +32092,7 @@
         <v>45064</v>
       </c>
       <c r="M396" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(A395=A396,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32119,7 +32131,7 @@
         <v>45064</v>
       </c>
       <c r="M397" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(A396=A397,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32158,7 +32170,7 @@
         <v>45064</v>
       </c>
       <c r="M398" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(A397=A398,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32197,7 +32209,7 @@
         <v>45064</v>
       </c>
       <c r="M399" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(A398=A399,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32236,7 +32248,7 @@
         <v>45064</v>
       </c>
       <c r="M400" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(A399=A400,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32275,7 +32287,7 @@
         <v>45064</v>
       </c>
       <c r="M401" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(A400=A401,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32317,7 +32329,7 @@
         <v>45064</v>
       </c>
       <c r="M402" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(A401=A402,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32356,7 +32368,7 @@
         <v>45064</v>
       </c>
       <c r="M403" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(A402=A403,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32395,7 +32407,7 @@
         <v>45064</v>
       </c>
       <c r="M404" t="str">
-        <f t="shared" si="6"/>
+        <f>IF(A403=A404,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32437,7 +32449,7 @@
         <v>45064</v>
       </c>
       <c r="M405" t="str">
-        <f t="shared" ref="M405:M435" si="7">IF(A404=A405,"dup","")</f>
+        <f>IF(A404=A405,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32476,7 +32488,7 @@
         <v>45064</v>
       </c>
       <c r="M406" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A405=A406,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32515,7 +32527,7 @@
         <v>45064</v>
       </c>
       <c r="M407" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A406=A407,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32554,7 +32566,7 @@
         <v>45064</v>
       </c>
       <c r="M408" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A407=A408,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32596,7 +32608,7 @@
         <v>45064</v>
       </c>
       <c r="M409" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A408=A409,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32635,7 +32647,7 @@
         <v>45064</v>
       </c>
       <c r="M410" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A409=A410,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32674,7 +32686,7 @@
         <v>45064</v>
       </c>
       <c r="M411" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A410=A411,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32716,7 +32728,7 @@
         <v>45064</v>
       </c>
       <c r="M412" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A411=A412,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32758,7 +32770,7 @@
         <v>45064</v>
       </c>
       <c r="M413" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A412=A413,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32797,7 +32809,7 @@
         <v>45064</v>
       </c>
       <c r="M414" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A413=A414,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32839,7 +32851,7 @@
         <v>45064</v>
       </c>
       <c r="M415" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A414=A415,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32878,7 +32890,7 @@
         <v>45064</v>
       </c>
       <c r="M416" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A415=A416,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32917,7 +32929,7 @@
         <v>45064</v>
       </c>
       <c r="M417" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A416=A417,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32956,7 +32968,7 @@
         <v>45064</v>
       </c>
       <c r="M418" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A417=A418,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -32995,7 +33007,7 @@
         <v>45064</v>
       </c>
       <c r="M419" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A418=A419,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -33034,7 +33046,7 @@
         <v>45064</v>
       </c>
       <c r="M420" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A419=A420,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -33073,7 +33085,7 @@
         <v>45064</v>
       </c>
       <c r="M421" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A420=A421,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -33115,7 +33127,7 @@
         <v>45064</v>
       </c>
       <c r="M422" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A421=A422,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -33154,7 +33166,7 @@
         <v>45064</v>
       </c>
       <c r="M423" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A422=A423,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -33193,7 +33205,7 @@
         <v>45064</v>
       </c>
       <c r="M424" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A423=A424,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -33235,7 +33247,7 @@
         <v>45064</v>
       </c>
       <c r="M425" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A424=A425,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -33274,7 +33286,7 @@
         <v>45064</v>
       </c>
       <c r="M426" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A425=A426,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -33313,7 +33325,7 @@
         <v>45064</v>
       </c>
       <c r="M427" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A426=A427,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -33352,7 +33364,7 @@
         <v>45064</v>
       </c>
       <c r="M428" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A427=A428,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -33391,7 +33403,7 @@
         <v>45064</v>
       </c>
       <c r="M429" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A428=A429,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -33430,7 +33442,7 @@
         <v>45064</v>
       </c>
       <c r="M430" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A429=A430,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -33469,7 +33481,7 @@
         <v>45064</v>
       </c>
       <c r="M431" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A430=A431,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -33511,7 +33523,7 @@
         <v>45064</v>
       </c>
       <c r="M432" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A431=A432,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -33550,7 +33562,7 @@
         <v>45064</v>
       </c>
       <c r="M433" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A432=A433,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -33589,7 +33601,7 @@
         <v>45064</v>
       </c>
       <c r="M434" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A433=A434,"dup","")</f>
         <v/>
       </c>
     </row>
@@ -33628,13 +33640,13 @@
         <v>45064</v>
       </c>
       <c r="M435" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(A434=A435,"dup","")</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L436">
-    <sortCondition ref="A2:A436"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M435">
+    <sortCondition ref="A2:A435"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -33642,6 +33654,637 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8680B73-135A-AC49-ACF5-848DFF694F0F}">
+  <dimension ref="A1:N19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="23.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1291</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1292</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1293</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1294</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1296</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>1297</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>1429</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1430</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="4">
+        <v>42641</v>
+      </c>
+      <c r="C2" s="4">
+        <v>42653</v>
+      </c>
+      <c r="D2">
+        <v>401</v>
+      </c>
+      <c r="E2">
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J2" t="s">
+        <v>127</v>
+      </c>
+      <c r="K2" s="5">
+        <v>750000</v>
+      </c>
+      <c r="L2" s="4">
+        <v>43831</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1431</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3" s="4">
+        <v>42839</v>
+      </c>
+      <c r="C3" s="4">
+        <v>42870</v>
+      </c>
+      <c r="D3">
+        <v>408</v>
+      </c>
+      <c r="E3">
+        <v>63</v>
+      </c>
+      <c r="F3">
+        <v>63</v>
+      </c>
+      <c r="H3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3" t="s">
+        <v>236</v>
+      </c>
+      <c r="J3" t="s">
+        <v>237</v>
+      </c>
+      <c r="K3" s="5">
+        <v>550000</v>
+      </c>
+      <c r="L3" s="4">
+        <v>43831</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1431</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>287</v>
+      </c>
+      <c r="B4" s="4">
+        <v>42916</v>
+      </c>
+      <c r="C4" s="4">
+        <v>42937</v>
+      </c>
+      <c r="D4">
+        <v>402</v>
+      </c>
+      <c r="E4">
+        <v>1.2</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>2000</v>
+      </c>
+      <c r="H4" t="s">
+        <v>290</v>
+      </c>
+      <c r="I4" t="s">
+        <v>288</v>
+      </c>
+      <c r="J4" t="s">
+        <v>289</v>
+      </c>
+      <c r="K4" s="5">
+        <v>498506</v>
+      </c>
+      <c r="L4" s="4">
+        <v>43831</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1431</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>303</v>
+      </c>
+      <c r="B5" s="4">
+        <v>42963</v>
+      </c>
+      <c r="C5" s="4">
+        <v>42968</v>
+      </c>
+      <c r="D5">
+        <v>201</v>
+      </c>
+      <c r="E5">
+        <v>134</v>
+      </c>
+      <c r="F5">
+        <v>134</v>
+      </c>
+      <c r="H5" t="s">
+        <v>306</v>
+      </c>
+      <c r="I5" t="s">
+        <v>304</v>
+      </c>
+      <c r="J5" t="s">
+        <v>305</v>
+      </c>
+      <c r="K5" s="5">
+        <v>750000</v>
+      </c>
+      <c r="L5" s="4">
+        <v>43831</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1431</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>410</v>
+      </c>
+      <c r="B6" s="4">
+        <v>43180</v>
+      </c>
+      <c r="C6" s="4">
+        <v>43220</v>
+      </c>
+      <c r="D6">
+        <v>414</v>
+      </c>
+      <c r="E6">
+        <v>11.11</v>
+      </c>
+      <c r="F6">
+        <v>11</v>
+      </c>
+      <c r="G6">
+        <v>1100</v>
+      </c>
+      <c r="H6" t="s">
+        <v>164</v>
+      </c>
+      <c r="I6" t="s">
+        <v>372</v>
+      </c>
+      <c r="J6" t="s">
+        <v>411</v>
+      </c>
+      <c r="K6" s="5">
+        <v>450000</v>
+      </c>
+      <c r="L6" s="4">
+        <v>43831</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1431</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>792</v>
+      </c>
+      <c r="B7" s="4">
+        <v>43809</v>
+      </c>
+      <c r="C7" s="4">
+        <v>43859</v>
+      </c>
+      <c r="D7">
+        <v>407</v>
+      </c>
+      <c r="E7">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="F7">
+        <v>76</v>
+      </c>
+      <c r="G7">
+        <v>1000</v>
+      </c>
+      <c r="H7" t="s">
+        <v>795</v>
+      </c>
+      <c r="I7" t="s">
+        <v>793</v>
+      </c>
+      <c r="J7" t="s">
+        <v>794</v>
+      </c>
+      <c r="K7" s="5">
+        <v>550000</v>
+      </c>
+      <c r="L7" s="4">
+        <v>43831</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1431</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>611</v>
+      </c>
+      <c r="B8" s="4">
+        <v>43594</v>
+      </c>
+      <c r="C8" s="4">
+        <v>43598</v>
+      </c>
+      <c r="D8">
+        <v>403</v>
+      </c>
+      <c r="E8">
+        <v>44</v>
+      </c>
+      <c r="F8">
+        <v>44</v>
+      </c>
+      <c r="H8" t="s">
+        <v>565</v>
+      </c>
+      <c r="I8" t="s">
+        <v>563</v>
+      </c>
+      <c r="J8" t="s">
+        <v>612</v>
+      </c>
+      <c r="K8" s="5">
+        <v>900000</v>
+      </c>
+      <c r="L8" s="4">
+        <v>43831</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1431</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>665</v>
+      </c>
+      <c r="B9" s="4">
+        <v>43647</v>
+      </c>
+      <c r="C9" s="4">
+        <v>43671</v>
+      </c>
+      <c r="D9">
+        <v>401</v>
+      </c>
+      <c r="E9">
+        <v>77</v>
+      </c>
+      <c r="F9">
+        <v>77</v>
+      </c>
+      <c r="H9" t="s">
+        <v>574</v>
+      </c>
+      <c r="I9" t="s">
+        <v>666</v>
+      </c>
+      <c r="J9" t="s">
+        <v>667</v>
+      </c>
+      <c r="K9" s="5">
+        <v>1200000</v>
+      </c>
+      <c r="L9" s="4">
+        <v>43831</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1431</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>692</v>
+      </c>
+      <c r="B10" s="4">
+        <v>43699</v>
+      </c>
+      <c r="C10" s="4">
+        <v>43699</v>
+      </c>
+      <c r="D10">
+        <v>405</v>
+      </c>
+      <c r="E10">
+        <v>42.2</v>
+      </c>
+      <c r="F10">
+        <v>42</v>
+      </c>
+      <c r="G10">
+        <v>2000</v>
+      </c>
+      <c r="H10" t="s">
+        <v>695</v>
+      </c>
+      <c r="I10" t="s">
+        <v>693</v>
+      </c>
+      <c r="J10" t="s">
+        <v>694</v>
+      </c>
+      <c r="K10" s="5">
+        <v>1850000</v>
+      </c>
+      <c r="L10" s="4">
+        <v>43831</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1431</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>946</v>
+      </c>
+      <c r="B11" s="4">
+        <v>44117</v>
+      </c>
+      <c r="C11" s="4">
+        <v>44118</v>
+      </c>
+      <c r="D11">
+        <v>201</v>
+      </c>
+      <c r="E11">
+        <v>31.1</v>
+      </c>
+      <c r="F11">
+        <v>31</v>
+      </c>
+      <c r="G11">
+        <v>1000</v>
+      </c>
+      <c r="H11" t="s">
+        <v>949</v>
+      </c>
+      <c r="I11" t="s">
+        <v>947</v>
+      </c>
+      <c r="J11" t="s">
+        <v>948</v>
+      </c>
+      <c r="K11" s="5">
+        <v>789000</v>
+      </c>
+      <c r="L11" s="4">
+        <v>43831</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1431</v>
+      </c>
+      <c r="N11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B12" s="4">
+        <v>44650</v>
+      </c>
+      <c r="C12" s="4">
+        <v>44671</v>
+      </c>
+      <c r="D12">
+        <v>407</v>
+      </c>
+      <c r="E12">
+        <v>58.1</v>
+      </c>
+      <c r="F12">
+        <v>58</v>
+      </c>
+      <c r="G12">
+        <v>1000</v>
+      </c>
+      <c r="H12" t="s">
+        <v>1246</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1244</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1245</v>
+      </c>
+      <c r="K12" s="5">
+        <v>1150000</v>
+      </c>
+      <c r="L12" s="4">
+        <v>43831</v>
+      </c>
+      <c r="M12" t="s">
+        <v>1431</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B13" s="4">
+        <v>44820</v>
+      </c>
+      <c r="C13" s="4">
+        <v>44851</v>
+      </c>
+      <c r="D13">
+        <v>408</v>
+      </c>
+      <c r="E13">
+        <v>19</v>
+      </c>
+      <c r="F13">
+        <v>19</v>
+      </c>
+      <c r="H13" t="s">
+        <v>1320</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1368</v>
+      </c>
+      <c r="J13" t="s">
+        <v>289</v>
+      </c>
+      <c r="K13" s="5">
+        <v>800000</v>
+      </c>
+      <c r="L13" s="4">
+        <v>45064</v>
+      </c>
+      <c r="M13" t="s">
+        <v>1431</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B14" s="4">
+        <v>44832</v>
+      </c>
+      <c r="C14" s="4">
+        <v>44900</v>
+      </c>
+      <c r="D14">
+        <v>408</v>
+      </c>
+      <c r="E14">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="F14">
+        <v>67</v>
+      </c>
+      <c r="G14">
+        <v>1000</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1390</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1388</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1389</v>
+      </c>
+      <c r="K14" s="5">
+        <v>510000</v>
+      </c>
+      <c r="L14" s="4">
+        <v>45064</v>
+      </c>
+      <c r="M14" t="s">
+        <v>1431</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N15">
+        <f>SUM(N2:N14)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N28">
+    <sortCondition ref="A2:A28"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E71A71-C623-7D42-B37F-2D49C69E3B06}">
   <dimension ref="A1:K76"/>
   <sheetViews>

</xml_diff>